<commit_message>
generate new data set
</commit_message>
<xml_diff>
--- a/data/Input/2025ClassEnrollCap.xlsx
+++ b/data/Input/2025ClassEnrollCap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CE6CFA-0BCA-7B48-BCB9-B1DAF75E9D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7C8AA-9C88-1E49-8DE1-E4F4435D3312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{7A323A41-FA22-704A-A51F-A23B5680A87B}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>Sec #</t>
   </si>
   <si>
-    <t>Enroll cap</t>
+    <t>Enroll Cap</t>
   </si>
 </sst>
 </file>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2841CFD7-7DC3-B04C-8B6C-E4C005B1DB9A}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix input for 2025 Courses
</commit_message>
<xml_diff>
--- a/data/Input/2025ClassEnrollCap.xlsx
+++ b/data/Input/2025ClassEnrollCap.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7C8AA-9C88-1E49-8DE1-E4F4435D3312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C032F0-A016-B142-9FB8-F98BED582C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{7A323A41-FA22-704A-A51F-A23B5680A87B}"/>
+    <workbookView xWindow="8720" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{7A323A41-FA22-704A-A51F-A23B5680A87B}"/>
   </bookViews>
   <sheets>
     <sheet name="2025Fall" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025Fall'!$A$1:$C$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025Fall'!$A$1:$C$72</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2841CFD7-7DC3-B04C-8B6C-E4C005B1DB9A}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="134" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,13 +758,13 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>541</v>
+        <v>550</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2">
-        <v>45</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -772,18 +772,18 @@
         <v>550</v>
       </c>
       <c r="B32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="B33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2">
         <v>120</v>
@@ -791,18 +791,18 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="2">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>775</v>
+        <v>790</v>
       </c>
       <c r="B49" s="2">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="C49" s="2">
         <v>30</v>
@@ -970,10 +970,10 @@
         <v>790</v>
       </c>
       <c r="B50" s="2">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C50" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -981,10 +981,10 @@
         <v>790</v>
       </c>
       <c r="B51" s="2">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C51" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -992,10 +992,10 @@
         <v>790</v>
       </c>
       <c r="B52" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C52" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1003,10 +1003,10 @@
         <v>790</v>
       </c>
       <c r="B53" s="2">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C53" s="2">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1014,10 +1014,10 @@
         <v>790</v>
       </c>
       <c r="B54" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C54" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1025,7 +1025,7 @@
         <v>790</v>
       </c>
       <c r="B55" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C55" s="2">
         <v>25</v>
@@ -1036,7 +1036,7 @@
         <v>790</v>
       </c>
       <c r="B56" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C56" s="2">
         <v>25</v>
@@ -1047,10 +1047,10 @@
         <v>790</v>
       </c>
       <c r="B57" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C57" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1058,22 +1058,16 @@
         <v>790</v>
       </c>
       <c r="B58" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C58" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>790</v>
-      </c>
-      <c r="B59" s="2">
-        <v>189</v>
-      </c>
-      <c r="C59" s="2">
-        <v>40</v>
-      </c>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
@@ -1085,10 +1079,10 @@
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
@@ -1135,16 +1129,12 @@
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C73" xr:uid="{2841CFD7-7DC3-B04C-8B6C-E4C005B1DB9A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
-    <sortCondition ref="A2:A73"/>
+  <autoFilter ref="A1:C72" xr:uid="{2841CFD7-7DC3-B04C-8B6C-E4C005B1DB9A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C72">
+    <sortCondition ref="A2:A72"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>